<commit_message>
Additions to terminating errors spreadsheet
</commit_message>
<xml_diff>
--- a/ErrorHandling/WorkInProgress_ErrorHandling/KnownTerminatingErrors.xlsx
+++ b/ErrorHandling/WorkInProgress_ErrorHandling/KnownTerminatingErrors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Cmdlet Name</t>
   </si>
@@ -81,6 +81,57 @@
   </si>
   <si>
     <t>You use the -CimSession or -PSSession parameters without also using the  -ListAvailable switch.</t>
+  </si>
+  <si>
+    <t>Where-Object</t>
+  </si>
+  <si>
+    <t>You attempt to use the -match or -notmatch operators (including all case sensitive versions) in Restricted Language mode.</t>
+  </si>
+  <si>
+    <t>Clear-History</t>
+  </si>
+  <si>
+    <t>You specify a -Count argument of less than 0.</t>
+  </si>
+  <si>
+    <t>New-PSSessionConfigurationFile</t>
+  </si>
+  <si>
+    <t>One of the values passed to the ModulesToImport parameter is not a string and not a hashtable.</t>
+  </si>
+  <si>
+    <t>You pass a value to the -Path parameter which is not on the file system provider, or does not end in .pssc</t>
+  </si>
+  <si>
+    <t>Set-PSSessionConfiguration</t>
+  </si>
+  <si>
+    <t>Export-PSSession</t>
+  </si>
+  <si>
+    <t>Start-Job</t>
+  </si>
+  <si>
+    <t>You attempt to use the -ScriptBlock or -InitializationScript parameters in a Constrained Language session (unless the "System Lockdown Policy" is set to "Enforce"; not sure what that logic is for.)</t>
+  </si>
+  <si>
+    <t>You specify the -OutputModule parameter, do not specify the -Force switch, and the directory passed to -OutputModule already exists.</t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
+    <t>Invoke-History</t>
+  </si>
+  <si>
+    <t>You pipe multiple values to the -Id parameter.</t>
+  </si>
+  <si>
+    <t>Wait-Job</t>
+  </si>
+  <si>
+    <t>Haven't finished analyzing this logic yet.  If the number of finished + blocked jobs doesn't match the number of jobs the cmdlet is monitoring, it will wind up throwing a terminating error.  (Not sure what can lead to that condition yet.)</t>
   </si>
 </sst>
 </file>
@@ -436,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -463,11 +514,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,6 +638,105 @@
         <v>18</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>